<commit_message>
cập nhật công việc
</commit_message>
<xml_diff>
--- a/Linux/06.NetBox/Tools/Import/sample_input.xlsx
+++ b/Linux/06.NetBox/Tools/Import/sample_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\A41488\Device Import Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Thuc-Tap\Linux\06.NetBox\Tools\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76445116-9ECA-4946-8A7B-5E71FD8CB8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F072A561-9646-496C-8342-5B4631C23FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{51D8CE69-D48F-4D47-B5F1-87CE3E7BE717}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Contract Number</t>
   </si>
   <si>
-    <t>Device Type</t>
-  </si>
-  <si>
     <t>Serial Number</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>ABC123D5</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -369,61 +369,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -764,7 +764,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,60 +798,60 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6">
         <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="K2" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6">
         <v>41</v>
@@ -868,272 +868,290 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6">
         <v>40</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6">
         <v>39</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="K5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="6">
         <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="6">
         <v>37</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>25</v>
+      <c r="K7" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6">
         <v>36</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="15"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="6">
         <v>35</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="30"/>
+      <c r="I9" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>25</v>
+      <c r="K9" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="6">
         <v>34</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="15"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6">
         <v>33</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="F11" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="G11" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>25</v>
+      <c r="H11" s="15"/>
+      <c r="I11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6">
         <v>32</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="29"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="6">
         <v>31</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="25"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="15"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="H11:H13"/>
     <mergeCell ref="J11:J13"/>
@@ -1143,24 +1161,6 @@
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="G11:G13"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>